<commit_message>
name changes for files
</commit_message>
<xml_diff>
--- a/simulation results/CI results.xlsx
+++ b/simulation results/CI results.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xijuan/local-fit-indices2/simulation results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E979B18D-F53E-8945-9D95-8B3F03371342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8BD59B-302C-0547-9D87-3B617FF379A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{98DFA7B3-F062-B349-9182-48BD3FB1DF62}"/>
+    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{98DFA7B3-F062-B349-9182-48BD3FB1DF62}"/>
   </bookViews>
   <sheets>
     <sheet name="RMSEA orig" sheetId="1" r:id="rId1"/>
     <sheet name="RMSEA high" sheetId="2" r:id="rId2"/>
+    <sheet name="SRMR orig" sheetId="3" r:id="rId3"/>
+    <sheet name="SRMR high" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="15">
   <si>
     <t>$n150</t>
   </si>
@@ -1017,7 +1019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C0D6F3-DF56-CB4B-8B63-EE9A098F541C}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -1593,4 +1595,1162 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D7461B5-2DD4-5448-A167-FD7595772993}">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>0.1175162</v>
+      </c>
+      <c r="C3">
+        <v>0.43851129999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.55440940000000005</v>
+      </c>
+      <c r="E3">
+        <v>0.60133499999999995</v>
+      </c>
+      <c r="F3">
+        <v>0.59000810000000004</v>
+      </c>
+      <c r="G3">
+        <v>0.59567150000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>0.87297729999999996</v>
+      </c>
+      <c r="C4">
+        <v>0.96278319999999995</v>
+      </c>
+      <c r="D4">
+        <v>0.91646439999999996</v>
+      </c>
+      <c r="E4">
+        <v>0.89583330000000005</v>
+      </c>
+      <c r="F4">
+        <v>0.89279940000000002</v>
+      </c>
+      <c r="G4">
+        <v>0.90736249999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>0.94174760000000002</v>
+      </c>
+      <c r="C5">
+        <v>0.98300969999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.95631069999999996</v>
+      </c>
+      <c r="E5">
+        <v>0.91828480000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.92354369999999997</v>
+      </c>
+      <c r="G5">
+        <v>0.92293689999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0.1175162</v>
+      </c>
+      <c r="C9">
+        <v>0.43851129999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.55440940000000005</v>
+      </c>
+      <c r="E9">
+        <v>0.60133499999999995</v>
+      </c>
+      <c r="F9">
+        <v>0.59000810000000004</v>
+      </c>
+      <c r="G9">
+        <v>0.59567150000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>0.87297729999999996</v>
+      </c>
+      <c r="C10">
+        <v>0.96278319999999995</v>
+      </c>
+      <c r="D10">
+        <v>0.91646439999999996</v>
+      </c>
+      <c r="E10">
+        <v>0.89583330000000005</v>
+      </c>
+      <c r="F10">
+        <v>0.89279940000000002</v>
+      </c>
+      <c r="G10">
+        <v>0.90736249999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>0.94174760000000002</v>
+      </c>
+      <c r="C11">
+        <v>0.98300969999999999</v>
+      </c>
+      <c r="D11">
+        <v>0.95631069999999996</v>
+      </c>
+      <c r="E11">
+        <v>0.91828480000000001</v>
+      </c>
+      <c r="F11">
+        <v>0.92354369999999997</v>
+      </c>
+      <c r="G11">
+        <v>0.92293689999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>0.11113339999999999</v>
+      </c>
+      <c r="C15">
+        <v>0.50640770000000002</v>
+      </c>
+      <c r="D15">
+        <v>0.57949539999999999</v>
+      </c>
+      <c r="E15">
+        <v>0.60652779999999995</v>
+      </c>
+      <c r="F15">
+        <v>0.59010810000000002</v>
+      </c>
+      <c r="G15">
+        <v>0.59251100000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>0.87244690000000003</v>
+      </c>
+      <c r="C16">
+        <v>0.9595515</v>
+      </c>
+      <c r="D16">
+        <v>0.8992791</v>
+      </c>
+      <c r="E16">
+        <v>0.92190629999999996</v>
+      </c>
+      <c r="F16">
+        <v>0.9014818</v>
+      </c>
+      <c r="G16">
+        <v>0.91950339999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>0.91810170000000002</v>
+      </c>
+      <c r="C17">
+        <v>0.9757709</v>
+      </c>
+      <c r="D17">
+        <v>0.91589909999999997</v>
+      </c>
+      <c r="E17">
+        <v>0.9389267</v>
+      </c>
+      <c r="F17">
+        <v>0.92010409999999998</v>
+      </c>
+      <c r="G17">
+        <v>0.9419303</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>0.1186</v>
+      </c>
+      <c r="C21">
+        <v>0.55659999999999998</v>
+      </c>
+      <c r="D21">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="E21">
+        <v>0.5988</v>
+      </c>
+      <c r="F21">
+        <v>0.59819999999999995</v>
+      </c>
+      <c r="G21">
+        <v>0.57440000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>0.87439999999999996</v>
+      </c>
+      <c r="C22">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="D22">
+        <v>0.92120000000000002</v>
+      </c>
+      <c r="E22">
+        <v>0.92359999999999998</v>
+      </c>
+      <c r="F22">
+        <v>0.91279999999999994</v>
+      </c>
+      <c r="G22">
+        <v>0.9204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <v>0.89839999999999998</v>
+      </c>
+      <c r="C23">
+        <v>0.96560000000000001</v>
+      </c>
+      <c r="D23">
+        <v>0.93940000000000001</v>
+      </c>
+      <c r="E23">
+        <v>0.94220000000000004</v>
+      </c>
+      <c r="F23">
+        <v>0.93240000000000001</v>
+      </c>
+      <c r="G23">
+        <v>0.93979999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>0.12139999999999999</v>
+      </c>
+      <c r="C27">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="D27">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="E27">
+        <v>0.60040000000000004</v>
+      </c>
+      <c r="F27">
+        <v>0.59919999999999995</v>
+      </c>
+      <c r="G27">
+        <v>0.58399999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>0.86260000000000003</v>
+      </c>
+      <c r="C28">
+        <v>0.89559999999999995</v>
+      </c>
+      <c r="D28">
+        <v>0.92179999999999995</v>
+      </c>
+      <c r="E28">
+        <v>0.92479999999999996</v>
+      </c>
+      <c r="F28">
+        <v>0.91080000000000005</v>
+      </c>
+      <c r="G28">
+        <v>0.91979999999999995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>0.87980000000000003</v>
+      </c>
+      <c r="C29">
+        <v>0.91420000000000001</v>
+      </c>
+      <c r="D29">
+        <v>0.93779999999999997</v>
+      </c>
+      <c r="E29">
+        <v>0.94379999999999997</v>
+      </c>
+      <c r="F29">
+        <v>0.93259999999999998</v>
+      </c>
+      <c r="G29">
+        <v>0.93940000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33">
+        <v>0.1172</v>
+      </c>
+      <c r="C33">
+        <v>0.56079999999999997</v>
+      </c>
+      <c r="D33">
+        <v>0.61980000000000002</v>
+      </c>
+      <c r="E33">
+        <v>0.5978</v>
+      </c>
+      <c r="F33">
+        <v>0.5968</v>
+      </c>
+      <c r="G33">
+        <v>0.59519999999999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34">
+        <v>0.86619999999999997</v>
+      </c>
+      <c r="C34">
+        <v>0.87</v>
+      </c>
+      <c r="D34">
+        <v>0.92520000000000002</v>
+      </c>
+      <c r="E34">
+        <v>0.92079999999999995</v>
+      </c>
+      <c r="F34">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="G34">
+        <v>0.92079999999999995</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35">
+        <v>0.88180000000000003</v>
+      </c>
+      <c r="C35">
+        <v>0.88719999999999999</v>
+      </c>
+      <c r="D35">
+        <v>0.94140000000000001</v>
+      </c>
+      <c r="E35">
+        <v>0.93979999999999997</v>
+      </c>
+      <c r="F35">
+        <v>0.93259999999999998</v>
+      </c>
+      <c r="G35">
+        <v>0.94279999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{065043F0-EFDA-7C4B-A63F-CB8FBD2FA76F}">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="C3">
+        <v>0.80979999999999996</v>
+      </c>
+      <c r="D3">
+        <v>0.8488</v>
+      </c>
+      <c r="E3">
+        <v>0.8266</v>
+      </c>
+      <c r="F3">
+        <v>0.83720000000000006</v>
+      </c>
+      <c r="G3">
+        <v>0.82679999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>0.87080000000000002</v>
+      </c>
+      <c r="C4">
+        <v>0.95420000000000005</v>
+      </c>
+      <c r="D4">
+        <v>0.91720000000000002</v>
+      </c>
+      <c r="E4">
+        <v>0.92020000000000002</v>
+      </c>
+      <c r="F4">
+        <v>0.9224</v>
+      </c>
+      <c r="G4">
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>0.87260000000000004</v>
+      </c>
+      <c r="C5">
+        <v>0.95679999999999998</v>
+      </c>
+      <c r="D5">
+        <v>0.92220000000000002</v>
+      </c>
+      <c r="E5">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="F5">
+        <v>0.92279999999999995</v>
+      </c>
+      <c r="G5">
+        <v>0.92859999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="C9">
+        <v>0.80979999999999996</v>
+      </c>
+      <c r="D9">
+        <v>0.8488</v>
+      </c>
+      <c r="E9">
+        <v>0.8266</v>
+      </c>
+      <c r="F9">
+        <v>0.83720000000000006</v>
+      </c>
+      <c r="G9">
+        <v>0.82679999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>0.87080000000000002</v>
+      </c>
+      <c r="C10">
+        <v>0.95420000000000005</v>
+      </c>
+      <c r="D10">
+        <v>0.91720000000000002</v>
+      </c>
+      <c r="E10">
+        <v>0.92020000000000002</v>
+      </c>
+      <c r="F10">
+        <v>0.9224</v>
+      </c>
+      <c r="G10">
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>0.87260000000000004</v>
+      </c>
+      <c r="C11">
+        <v>0.95679999999999998</v>
+      </c>
+      <c r="D11">
+        <v>0.92220000000000002</v>
+      </c>
+      <c r="E11">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="F11">
+        <v>0.92279999999999995</v>
+      </c>
+      <c r="G11">
+        <v>0.92859999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>0.57140000000000002</v>
+      </c>
+      <c r="C15">
+        <v>0.7954</v>
+      </c>
+      <c r="D15">
+        <v>0.84519999999999995</v>
+      </c>
+      <c r="E15">
+        <v>0.83320000000000005</v>
+      </c>
+      <c r="F15">
+        <v>0.8296</v>
+      </c>
+      <c r="G15">
+        <v>0.82220000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>0.87539999999999996</v>
+      </c>
+      <c r="C16">
+        <v>0.90139999999999998</v>
+      </c>
+      <c r="D16">
+        <v>0.9284</v>
+      </c>
+      <c r="E16">
+        <v>0.92420000000000002</v>
+      </c>
+      <c r="F16">
+        <v>0.92</v>
+      </c>
+      <c r="G16">
+        <v>0.9204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>0.875</v>
+      </c>
+      <c r="C17">
+        <v>0.9032</v>
+      </c>
+      <c r="D17">
+        <v>0.93159999999999998</v>
+      </c>
+      <c r="E17">
+        <v>0.92959999999999998</v>
+      </c>
+      <c r="F17">
+        <v>0.92459999999999998</v>
+      </c>
+      <c r="G17">
+        <v>0.9264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>0.57920000000000005</v>
+      </c>
+      <c r="C21">
+        <v>0.78720000000000001</v>
+      </c>
+      <c r="D21">
+        <v>0.84179999999999999</v>
+      </c>
+      <c r="E21">
+        <v>0.81440000000000001</v>
+      </c>
+      <c r="F21">
+        <v>0.82040000000000002</v>
+      </c>
+      <c r="G21">
+        <v>0.81459999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>0.86819999999999997</v>
+      </c>
+      <c r="C22">
+        <v>0.87180000000000002</v>
+      </c>
+      <c r="D22">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="E22">
+        <v>0.91779999999999995</v>
+      </c>
+      <c r="F22">
+        <v>0.91459999999999997</v>
+      </c>
+      <c r="G22">
+        <v>0.91859999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <v>0.87260000000000004</v>
+      </c>
+      <c r="C23">
+        <v>0.877</v>
+      </c>
+      <c r="D23">
+        <v>0.92720000000000002</v>
+      </c>
+      <c r="E23">
+        <v>0.92359999999999998</v>
+      </c>
+      <c r="F23">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="G23">
+        <v>0.92679999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="C27">
+        <v>0.79379999999999995</v>
+      </c>
+      <c r="D27">
+        <v>0.83460000000000001</v>
+      </c>
+      <c r="E27">
+        <v>0.81759999999999999</v>
+      </c>
+      <c r="F27">
+        <v>0.81640000000000001</v>
+      </c>
+      <c r="G27">
+        <v>0.80579999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>0.85960000000000003</v>
+      </c>
+      <c r="C28">
+        <v>0.88780000000000003</v>
+      </c>
+      <c r="D28">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="E28">
+        <v>0.91920000000000002</v>
+      </c>
+      <c r="F28">
+        <v>0.91679999999999995</v>
+      </c>
+      <c r="G28">
+        <v>0.91520000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>0.86040000000000005</v>
+      </c>
+      <c r="C29">
+        <v>0.89239999999999997</v>
+      </c>
+      <c r="D29">
+        <v>0.92759999999999998</v>
+      </c>
+      <c r="E29">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="F29">
+        <v>0.9234</v>
+      </c>
+      <c r="G29">
+        <v>0.92379999999999995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="C33">
+        <v>0.79020000000000001</v>
+      </c>
+      <c r="D33">
+        <v>0.82820000000000005</v>
+      </c>
+      <c r="E33">
+        <v>0.82079999999999997</v>
+      </c>
+      <c r="F33">
+        <v>0.82179999999999997</v>
+      </c>
+      <c r="G33">
+        <v>0.80959999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34">
+        <v>0.86419999999999997</v>
+      </c>
+      <c r="C34">
+        <v>0.89559999999999995</v>
+      </c>
+      <c r="D34">
+        <v>0.91879999999999995</v>
+      </c>
+      <c r="E34">
+        <v>0.91379999999999995</v>
+      </c>
+      <c r="F34">
+        <v>0.91979999999999995</v>
+      </c>
+      <c r="G34">
+        <v>0.91900000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35">
+        <v>0.86160000000000003</v>
+      </c>
+      <c r="C35">
+        <v>0.89780000000000004</v>
+      </c>
+      <c r="D35">
+        <v>0.92559999999999998</v>
+      </c>
+      <c r="E35">
+        <v>0.92179999999999995</v>
+      </c>
+      <c r="F35">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="G35">
+        <v>0.92759999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>